<commit_message>
Transfer from cashflow now correctly sets the remaining cashflow amount
</commit_message>
<xml_diff>
--- a/tests/Feature/config/cashflow_transfer_zero.xlsx
+++ b/tests/Feature/config/cashflow_transfer_zero.xlsx
@@ -176,55 +176,55 @@
     <t>income</t>
   </si>
   <si>
-    <t xml:space="preserve">Incometransfered -240000 + 0 (tax) = 240000 to fond.2022.asset.marketAmount </t>
+    <t xml:space="preserve">Incometransfered -240000 + 0 (tax) = 240000 to fond.2022.asset.marketAmount  transfer 240000 (100% of 240000=240000) to fond.2022.asset.marketAmount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered -240000 + 0 (tax) = 240000 to fond.2023.asset.marketAmount </t>
+    <t xml:space="preserve">transfered -240000 + 0 (tax) = 240000 to fond.2023.asset.marketAmount  transfer 240000 (100% of 240000=240000) to fond.2023.asset.marketAmount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered -240000 + 0 (tax) = 240000 to fond.2024.asset.marketAmount </t>
+    <t xml:space="preserve">transfered -240000 + 0 (tax) = 240000 to fond.2024.asset.marketAmount  transfer 240000 (100% of 240000=240000) to fond.2024.asset.marketAmount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered -240000 + 0 (tax) = 240000 to fond.2025.asset.marketAmount </t>
+    <t xml:space="preserve">transfered -240000 + 0 (tax) = 240000 to fond.2025.asset.marketAmount  transfer 240000 (100% of 240000=240000) to fond.2025.asset.marketAmount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered -240000 + 0 (tax) = 240000 to fond.2026.asset.marketAmount </t>
+    <t xml:space="preserve">transfered -240000 + 0 (tax) = 240000 to fond.2026.asset.marketAmount  transfer 240000 (100% of 240000=240000) to fond.2026.asset.marketAmount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered -240000 + 0 (tax) = 240000 to fond.2027.asset.marketAmount </t>
+    <t xml:space="preserve">transfered -240000 + 0 (tax) = 240000 to fond.2027.asset.marketAmount  transfer 240000 (100% of 240000=240000) to fond.2027.asset.marketAmount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered -240000 + 0 (tax) = 240000 to fond.2028.asset.marketAmount </t>
+    <t xml:space="preserve">transfered -240000 + 0 (tax) = 240000 to fond.2028.asset.marketAmount  transfer 240000 (100% of 240000=240000) to fond.2028.asset.marketAmount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered -240000 + 0 (tax) = 240000 to fond.2029.asset.marketAmount </t>
+    <t xml:space="preserve">transfered -240000 + 0 (tax) = 240000 to fond.2029.asset.marketAmount  transfer 240000 (100% of 240000=240000) to fond.2029.asset.marketAmount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered -240000 + 0 (tax) = 240000 to fond.2030.asset.marketAmount </t>
+    <t xml:space="preserve">transfered -240000 + 0 (tax) = 240000 to fond.2030.asset.marketAmount  transfer 240000 (100% of 240000=240000) to fond.2030.asset.marketAmount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered -240000 + 0 (tax) = 240000 to fond.2031.asset.marketAmount </t>
+    <t xml:space="preserve">transfered -240000 + 0 (tax) = 240000 to fond.2031.asset.marketAmount  transfer 240000 (100% of 240000=240000) to fond.2031.asset.marketAmount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered -240000 + 0 (tax) = 240000 to fond.2032.asset.marketAmount </t>
+    <t xml:space="preserve">transfered -240000 + 0 (tax) = 240000 to fond.2032.asset.marketAmount  transfer 240000 (100% of 240000=240000) to fond.2032.asset.marketAmount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered -240000 + 0 (tax) = 240000 to fond.2033.asset.marketAmount </t>
+    <t xml:space="preserve">transfered -240000 + 0 (tax) = 240000 to fond.2033.asset.marketAmount  transfer 240000 (100% of 240000=240000) to fond.2033.asset.marketAmount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered -240000 + 0 (tax) = 240000 to fond.2034.asset.marketAmount </t>
+    <t xml:space="preserve">transfered -240000 + 0 (tax) = 240000 to fond.2034.asset.marketAmount  transfer 240000 (100% of 240000=240000) to fond.2034.asset.marketAmount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered -240000 + 0 (tax) = 240000 to fond.2035.asset.marketAmount </t>
+    <t xml:space="preserve">transfered -240000 + 0 (tax) = 240000 to fond.2035.asset.marketAmount  transfer 240000 (100% of 240000=240000) to fond.2035.asset.marketAmount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered -240000 + 0 (tax) = 240000 to fond.2036.asset.marketAmount </t>
+    <t xml:space="preserve">transfered -240000 + 0 (tax) = 240000 to fond.2036.asset.marketAmount  transfer 240000 (100% of 240000=240000) to fond.2036.asset.marketAmount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered -240000 + 0 (tax) = 240000 to fond.2037.asset.marketAmount </t>
+    <t xml:space="preserve">transfered -240000 + 0 (tax) = 240000 to fond.2037.asset.marketAmount  transfer 240000 (100% of 240000=240000) to fond.2037.asset.marketAmount </t>
   </si>
   <si>
-    <t xml:space="preserve">Pensioned, no more salary from heretransfered -240000 + 0 (tax) = 240000 to fond.2038.asset.marketAmount </t>
+    <t xml:space="preserve">Pensioned, no more salary from heretransfered -240000 + 0 (tax) = 240000 to fond.2038.asset.marketAmount  transfer 240000 (100% of 240000=240000) to fond.2038.asset.marketAmount </t>
   </si>
   <si>
     <t>fond</t>
@@ -236,55 +236,55 @@
     <t xml:space="preserve"> Asset rule: </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2022.cashflow.afterTaxAmount  Asset rule: </t>
+    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2022.cashflow.afterTaxAmount  transfer 240000 (100% of 240000=240000) to fond.2022.asset.marketAmount  Asset rule: </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2023.cashflow.afterTaxAmount  Asset rule: </t>
+    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2023.cashflow.afterTaxAmount  transfer 240000 (100% of 240000=240000) to fond.2023.asset.marketAmount  Asset rule: </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2024.cashflow.afterTaxAmount  Asset rule: </t>
+    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2024.cashflow.afterTaxAmount  transfer 240000 (100% of 240000=240000) to fond.2024.asset.marketAmount  Asset rule: </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2025.cashflow.afterTaxAmount  Asset rule: </t>
+    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2025.cashflow.afterTaxAmount  transfer 240000 (100% of 240000=240000) to fond.2025.asset.marketAmount  Asset rule: </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2026.cashflow.afterTaxAmount  Asset rule: </t>
+    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2026.cashflow.afterTaxAmount  transfer 240000 (100% of 240000=240000) to fond.2026.asset.marketAmount  Asset rule: </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2027.cashflow.afterTaxAmount  Asset rule: </t>
+    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2027.cashflow.afterTaxAmount  transfer 240000 (100% of 240000=240000) to fond.2027.asset.marketAmount  Asset rule: </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2028.cashflow.afterTaxAmount  Asset rule: </t>
+    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2028.cashflow.afterTaxAmount  transfer 240000 (100% of 240000=240000) to fond.2028.asset.marketAmount  Asset rule: </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2029.cashflow.afterTaxAmount  Asset rule: </t>
+    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2029.cashflow.afterTaxAmount  transfer 240000 (100% of 240000=240000) to fond.2029.asset.marketAmount  Asset rule: </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2030.cashflow.afterTaxAmount  Asset rule: </t>
+    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2030.cashflow.afterTaxAmount  transfer 240000 (100% of 240000=240000) to fond.2030.asset.marketAmount  Asset rule: </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2031.cashflow.afterTaxAmount  Asset rule: </t>
+    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2031.cashflow.afterTaxAmount  transfer 240000 (100% of 240000=240000) to fond.2031.asset.marketAmount  Asset rule: </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2032.cashflow.afterTaxAmount  Asset rule: </t>
+    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2032.cashflow.afterTaxAmount  transfer 240000 (100% of 240000=240000) to fond.2032.asset.marketAmount  Asset rule: </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2033.cashflow.afterTaxAmount  Asset rule: </t>
+    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2033.cashflow.afterTaxAmount  transfer 240000 (100% of 240000=240000) to fond.2033.asset.marketAmount  Asset rule: </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2034.cashflow.afterTaxAmount  Asset rule: </t>
+    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2034.cashflow.afterTaxAmount  transfer 240000 (100% of 240000=240000) to fond.2034.asset.marketAmount  Asset rule: </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2035.cashflow.afterTaxAmount  Asset rule: </t>
+    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2035.cashflow.afterTaxAmount  transfer 240000 (100% of 240000=240000) to fond.2035.asset.marketAmount  Asset rule: </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2036.cashflow.afterTaxAmount  Asset rule: </t>
+    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2036.cashflow.afterTaxAmount  transfer 240000 (100% of 240000=240000) to fond.2036.asset.marketAmount  Asset rule: </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2037.cashflow.afterTaxAmount  Asset rule: </t>
+    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2037.cashflow.afterTaxAmount  transfer 240000 (100% of 240000=240000) to fond.2037.asset.marketAmount  Asset rule: </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2038.cashflow.afterTaxAmount  Asset rule: </t>
+    <t xml:space="preserve">transfered 240000 - 0 (tax) = 240000 from salary.2038.cashflow.afterTaxAmount  transfer 240000 (100% of 240000=240000) to fond.2038.asset.marketAmount  Asset rule: </t>
   </si>
   <si>
     <t>total</t>

</xml_diff>